<commit_message>
Añadida posibilidad de guardar informacion de a los usuarios que se recalifico
</commit_message>
<xml_diff>
--- a/datos/datos_recalificar_todo.xlsx
+++ b/datos/datos_recalificar_todo.xlsx
@@ -28,10 +28,10 @@
     <t xml:space="preserve">ACTIVIDAD</t>
   </si>
   <si>
-    <t xml:space="preserve">CPS1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CPS1.2</t>
+    <t xml:space="preserve">CPS1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPS1.4</t>
   </si>
 </sst>
 </file>
@@ -169,7 +169,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1:C3"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -198,7 +198,7 @@
       <c r="A3" s="1" t="n">
         <v>13317</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3"/>

</xml_diff>